<commit_message>
I|O -> IO for master
</commit_message>
<xml_diff>
--- a/sbus-to-ztex/signals.xlsx
+++ b/sbus-to-ztex/signals.xlsx
@@ -2931,6 +2931,11 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
+  <dxfs count="1">
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false" readingOrder="1"/>
+    </dxf>
+  </dxfs>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -3001,8 +3006,8 @@
   </sheetPr>
   <dimension ref="A1:AG231"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AB62" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AG93" activeCellId="0" sqref="AG93:AG95"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I83" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="V106" activeCellId="0" sqref="V106:V112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8925,7 +8930,7 @@
         <v>-49.2056541792</v>
       </c>
       <c r="T84" s="0" t="s">
-        <v>146</v>
+        <v>35</v>
       </c>
       <c r="U84" s="29" t="str">
         <f aca="false">IF(AND(K84&lt;&gt;"",K84&lt;&gt;"+3v3",K84&lt;&gt;"GND"),CONCATENATE("set_property PACKAGE_PIN ",D84," [get_ports {",K84,"}]",CHAR(10),"set_property IOSTANDARD LVTTL [get_ports {",K84,"}]",CHAR(10)),"")</f>
@@ -8945,7 +8950,8 @@
       <c r="Y84" s="7" t="str">
         <f aca="false">CONCATENATE(IF(OR(T84="IO",T84="I"),V84,""),IF(OR(T84="IO",T84="O"),W84,""))</f>
         <v>set_input_delay -clock SBUS_3V3_CLK -min 0.996 [get_ports {SBUS_3V3_SIZ[0]}]
-set_input_delay -clock SBUS_3V3_CLK -max 25.578 [get_ports {SBUS_3V3_SIZ[0]}]</v>
+set_input_delay -clock SBUS_3V3_CLK -max 25.578 [get_ports {SBUS_3V3_SIZ[0]}]set_output_delay -clock SBUS_3V3_CLK -min -1.580 [get_ports {SBUS_3V3_SIZ[0]}]
+set_output_delay -clock SBUS_3V3_CLK -max 21.727 [get_ports {SBUS_3V3_SIZ[0]}]</v>
       </c>
       <c r="AG84" s="8" t="str">
         <f aca="false">IF(OR(LEFT(K84,3)="LED",LEFT(K84,16)="SBUS_DATA_OE_LED"),CONCATENATE("(",CHAR(34),"user_led",CHAR(34),", 0, Pins(",CHAR(34),D84,CHAR(34),"),  IOStandard(",CHAR(34),"lvcmos33",CHAR(34),")), ",CHAR(35),K84),"")</f>
@@ -9313,7 +9319,7 @@
         <v>-34.27457333718</v>
       </c>
       <c r="T89" s="0" t="s">
-        <v>146</v>
+        <v>35</v>
       </c>
       <c r="U89" s="29" t="str">
         <f aca="false">IF(AND(K89&lt;&gt;"",K89&lt;&gt;"+3v3",K89&lt;&gt;"GND"),CONCATENATE("set_property PACKAGE_PIN ",D89," [get_ports {",K89,"}]",CHAR(10),"set_property IOSTANDARD LVTTL [get_ports {",K89,"}]",CHAR(10)),"")</f>
@@ -9333,7 +9339,8 @@
       <c r="Y89" s="7" t="str">
         <f aca="false">CONCATENATE(IF(OR(T89="IO",T89="I"),V89,""),IF(OR(T89="IO",T89="O"),W89,""))</f>
         <v>set_input_delay -clock SBUS_3V3_CLK -min 0.921 [get_ports {SBUS_3V3_SIZ[1]}]
-set_input_delay -clock SBUS_3V3_CLK -max 25.478 [get_ports {SBUS_3V3_SIZ[1]}]</v>
+set_input_delay -clock SBUS_3V3_CLK -max 25.478 [get_ports {SBUS_3V3_SIZ[1]}]set_output_delay -clock SBUS_3V3_CLK -min -1.655 [get_ports {SBUS_3V3_SIZ[1]}]
+set_output_delay -clock SBUS_3V3_CLK -max 21.627 [get_ports {SBUS_3V3_SIZ[1]}]</v>
       </c>
       <c r="AG89" s="8" t="str">
         <f aca="false">IF(OR(LEFT(K89,3)="LED",LEFT(K89,16)="SBUS_DATA_OE_LED"),CONCATENATE("(",CHAR(34),"user_led",CHAR(34),", 0, Pins(",CHAR(34),D89,CHAR(34),"),  IOStandard(",CHAR(34),"lvcmos33",CHAR(34),")), ",CHAR(35),K89),"")</f>
@@ -9460,7 +9467,7 @@
         <v>-36.4499228779</v>
       </c>
       <c r="T91" s="0" t="s">
-        <v>146</v>
+        <v>35</v>
       </c>
       <c r="U91" s="29" t="str">
         <f aca="false">IF(AND(K91&lt;&gt;"",K91&lt;&gt;"+3v3",K91&lt;&gt;"GND"),CONCATENATE("set_property PACKAGE_PIN ",D91," [get_ports {",K91,"}]",CHAR(10),"set_property IOSTANDARD LVTTL [get_ports {",K91,"}]",CHAR(10)),"")</f>
@@ -9480,7 +9487,8 @@
       <c r="Y91" s="7" t="str">
         <f aca="false">CONCATENATE(IF(OR(T91="IO",T91="I"),V91,""),IF(OR(T91="IO",T91="O"),W91,""))</f>
         <v>set_input_delay -clock SBUS_3V3_CLK -min 0.932 [get_ports {SBUS_3V3_SIZ[2]}]
-set_input_delay -clock SBUS_3V3_CLK -max 25.493 [get_ports {SBUS_3V3_SIZ[2]}]</v>
+set_input_delay -clock SBUS_3V3_CLK -max 25.493 [get_ports {SBUS_3V3_SIZ[2]}]set_output_delay -clock SBUS_3V3_CLK -min -1.644 [get_ports {SBUS_3V3_SIZ[2]}]
+set_output_delay -clock SBUS_3V3_CLK -max 21.641 [get_ports {SBUS_3V3_SIZ[2]}]</v>
       </c>
       <c r="AG91" s="8" t="str">
         <f aca="false">IF(OR(LEFT(K91,3)="LED",LEFT(K91,16)="SBUS_DATA_OE_LED"),CONCATENATE("(",CHAR(34),"user_led",CHAR(34),", 0, Pins(",CHAR(34),D91,CHAR(34),"),  IOStandard(",CHAR(34),"lvcmos33",CHAR(34),")), ",CHAR(35),K91),"")</f>
@@ -9538,7 +9546,7 @@
         <v>-35.3359455394</v>
       </c>
       <c r="T92" s="0" t="s">
-        <v>264</v>
+        <v>35</v>
       </c>
       <c r="U92" s="29" t="str">
         <f aca="false">IF(AND(K92&lt;&gt;"",K92&lt;&gt;"+3v3",K92&lt;&gt;"GND"),CONCATENATE("set_property PACKAGE_PIN ",D92," [get_ports {",K92,"}]",CHAR(10),"set_property IOSTANDARD LVTTL [get_ports {",K92,"}]",CHAR(10)),"")</f>
@@ -9557,7 +9565,8 @@
       </c>
       <c r="Y92" s="7" t="str">
         <f aca="false">CONCATENATE(IF(OR(T92="IO",T92="I"),V92,""),IF(OR(T92="IO",T92="O"),W92,""))</f>
-        <v>set_output_delay -clock SBUS_3V3_CLK -min -1.649 [get_ports {SBUS_3V3_EER*}]
+        <v>set_input_delay -clock SBUS_3V3_CLK -min 0.927 [get_ports {SBUS_3V3_EER*}]
+set_input_delay -clock SBUS_3V3_CLK -max 25.486 [get_ports {SBUS_3V3_EER*}]set_output_delay -clock SBUS_3V3_CLK -min -1.649 [get_ports {SBUS_3V3_EER*}]
 set_output_delay -clock SBUS_3V3_CLK -max 21.634 [get_ports {SBUS_3V3_EER*}]</v>
       </c>
       <c r="AG92" s="8" t="str">
@@ -10346,7 +10355,7 @@
         <v>-16.2581268424</v>
       </c>
       <c r="T104" s="0" t="s">
-        <v>146</v>
+        <v>35</v>
       </c>
       <c r="U104" s="6" t="str">
         <f aca="false">IF(AND(K104&lt;&gt;"",K104&lt;&gt;"+3v3",K104&lt;&gt;"GND"),CONCATENATE("set_property PACKAGE_PIN ",D104," [get_ports {",K104,"}]",CHAR(10),"set_property IOSTANDARD LVTTL [get_ports {",K104,"}]",CHAR(10)),"")</f>
@@ -10366,7 +10375,8 @@
       <c r="Y104" s="7" t="str">
         <f aca="false">CONCATENATE(IF(OR(T104="IO",T104="I"),V104,""),IF(OR(T104="IO",T104="O"),W104,""))</f>
         <v>set_input_delay -clock SBUS_3V3_CLK -min 0.831 [get_ports {SBUS_3V3_PPRD}]
-set_input_delay -clock SBUS_3V3_CLK -max 25.358 [get_ports {SBUS_3V3_PPRD}]</v>
+set_input_delay -clock SBUS_3V3_CLK -max 25.358 [get_ports {SBUS_3V3_PPRD}]set_output_delay -clock SBUS_3V3_CLK -min -1.745 [get_ports {SBUS_3V3_PPRD}]
+set_output_delay -clock SBUS_3V3_CLK -max 21.507 [get_ports {SBUS_3V3_PPRD}]</v>
       </c>
       <c r="AG104" s="8" t="str">
         <f aca="false">IF(OR(LEFT(K104,3)="LED",LEFT(K104,16)="SBUS_DATA_OE_LED"),CONCATENATE("(",CHAR(34),"user_led",CHAR(34),", 0, Pins(",CHAR(34),D104,CHAR(34),"),  IOStandard(",CHAR(34),"lvcmos33",CHAR(34),")), ",CHAR(35),K104),"")</f>
@@ -10493,7 +10503,7 @@
         <v>-16.6557223604</v>
       </c>
       <c r="T106" s="0" t="s">
-        <v>264</v>
+        <v>35</v>
       </c>
       <c r="U106" s="6" t="str">
         <f aca="false">IF(AND(K106&lt;&gt;"",K106&lt;&gt;"+3v3",K106&lt;&gt;"GND"),CONCATENATE("set_property PACKAGE_PIN ",D106," [get_ports {",K106,"}]",CHAR(10),"set_property IOSTANDARD LVTTL [get_ports {",K106,"}]",CHAR(10)),"")</f>
@@ -10512,7 +10522,8 @@
       </c>
       <c r="Y106" s="7" t="str">
         <f aca="false">CONCATENATE(IF(OR(T106="IO",T106="I"),V106,""),IF(OR(T106="IO",T106="O"),W106,""))</f>
-        <v>set_output_delay -clock SBUS_3V3_CLK -min -1.743 [get_ports {SBUS_3V3_ACK[0]*}]
+        <v>set_input_delay -clock SBUS_3V3_CLK -min 0.833 [get_ports {SBUS_3V3_ACK[0]*}]
+set_input_delay -clock SBUS_3V3_CLK -max 25.361 [get_ports {SBUS_3V3_ACK[0]*}]set_output_delay -clock SBUS_3V3_CLK -min -1.743 [get_ports {SBUS_3V3_ACK[0]*}]
 set_output_delay -clock SBUS_3V3_CLK -max 21.510 [get_ports {SBUS_3V3_ACK[0]*}]</v>
       </c>
       <c r="AG106" s="8" t="str">
@@ -10651,7 +10662,7 @@
         <v>-15.7736847187</v>
       </c>
       <c r="T108" s="0" t="s">
-        <v>264</v>
+        <v>35</v>
       </c>
       <c r="U108" s="29" t="str">
         <f aca="false">IF(AND(K108&lt;&gt;"",K108&lt;&gt;"+3v3",K108&lt;&gt;"GND"),CONCATENATE("set_property PACKAGE_PIN ",D108," [get_ports {",K108,"}]",CHAR(10),"set_property IOSTANDARD LVTTL [get_ports {",K108,"}]",CHAR(10)),"")</f>
@@ -10670,7 +10681,8 @@
       </c>
       <c r="Y108" s="7" t="str">
         <f aca="false">CONCATENATE(IF(OR(T108="IO",T108="I"),V108,""),IF(OR(T108="IO",T108="O"),W108,""))</f>
-        <v>set_output_delay -clock SBUS_3V3_CLK -min -1.747 [get_ports {SBUS_3V3_ACK[1]*}]
+        <v>set_input_delay -clock SBUS_3V3_CLK -min 0.829 [get_ports {SBUS_3V3_ACK[1]*}]
+set_input_delay -clock SBUS_3V3_CLK -max 25.355 [get_ports {SBUS_3V3_ACK[1]*}]set_output_delay -clock SBUS_3V3_CLK -min -1.747 [get_ports {SBUS_3V3_ACK[1]*}]
 set_output_delay -clock SBUS_3V3_CLK -max 21.504 [get_ports {SBUS_3V3_ACK[1]*}]</v>
       </c>
       <c r="AG108" s="8" t="str">
@@ -10936,7 +10948,7 @@
         <v>-9.70572909559999</v>
       </c>
       <c r="T112" s="0" t="s">
-        <v>264</v>
+        <v>35</v>
       </c>
       <c r="U112" s="29" t="str">
         <f aca="false">IF(AND(K112&lt;&gt;"",K112&lt;&gt;"+3v3",K112&lt;&gt;"GND"),CONCATENATE("set_property PACKAGE_PIN ",D112," [get_ports {",K112,"}]",CHAR(10),"set_property IOSTANDARD LVTTL [get_ports {",K112,"}]",CHAR(10)),"")</f>
@@ -10955,7 +10967,8 @@
       </c>
       <c r="Y112" s="7" t="str">
         <f aca="false">CONCATENATE(IF(OR(T112="IO",T112="I"),V112,""),IF(OR(T112="IO",T112="O"),W112,""))</f>
-        <v>set_output_delay -clock SBUS_3V3_CLK -min -1.778 [get_ports {SBUS_3V3_ACK[2]*}]
+        <v>set_input_delay -clock SBUS_3V3_CLK -min 0.799 [get_ports {SBUS_3V3_ACK[2]*}]
+set_input_delay -clock SBUS_3V3_CLK -max 25.315 [get_ports {SBUS_3V3_ACK[2]*}]set_output_delay -clock SBUS_3V3_CLK -min -1.778 [get_ports {SBUS_3V3_ACK[2]*}]
 set_output_delay -clock SBUS_3V3_CLK -max 21.463 [get_ports {SBUS_3V3_ACK[2]*}]</v>
       </c>
       <c r="AG112" s="8" t="str">
@@ -13708,7 +13721,7 @@
   <dimension ref="A4:C80"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A81" activeCellId="1" sqref="AG93:AG95 A81"/>
+      <selection pane="topLeft" activeCell="A81" activeCellId="1" sqref="V106:V112 A81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14585,7 +14598,7 @@
   <dimension ref="A1:B103"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B47" activeCellId="1" sqref="AG93:AG95 B47"/>
+      <selection pane="topLeft" activeCell="B47" activeCellId="1" sqref="V106:V112 B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -15412,7 +15425,7 @@
   <dimension ref="A1:H172"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G2" activeCellId="1" sqref="AG93:AG95 G2"/>
+      <selection pane="topLeft" activeCell="G2" activeCellId="1" sqref="V106:V112 G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>